<commit_message>
Version bump for scatacseq... submission fixtures still work
</commit_message>
<xml_diff>
--- a/docs/scatacseq/scatacseq-metadata.xlsx
+++ b/docs/scatacseq/scatacseq-metadata.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Export as TSV" sheetId="1" r:id="rId1"/>
-    <sheet name="assay_category list" sheetId="2" r:id="rId2"/>
-    <sheet name="assay_type list" sheetId="3" r:id="rId3"/>
-    <sheet name="analyte_class list" sheetId="4" r:id="rId4"/>
-    <sheet name="sc_isolation_entity list" sheetId="5" r:id="rId5"/>
-    <sheet name="sc_isolation_enrichment list" sheetId="6" r:id="rId6"/>
-    <sheet name="transposition_method list" sheetId="7" r:id="rId7"/>
-    <sheet name="transposition_...se_source list" sheetId="8" r:id="rId8"/>
-    <sheet name="library_layout list" sheetId="9" r:id="rId9"/>
-    <sheet name="library_final_yield_unit list" sheetId="10" r:id="rId10"/>
+    <sheet name="version list" sheetId="2" r:id="rId2"/>
+    <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
+    <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
+    <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
+    <sheet name="sc_isolation_entity list" sheetId="6" r:id="rId6"/>
+    <sheet name="sc_isolation_enrichment list" sheetId="7" r:id="rId7"/>
+    <sheet name="transposition_method list" sheetId="8" r:id="rId8"/>
+    <sheet name="transposition_...se_source list" sheetId="9" r:id="rId9"/>
+    <sheet name="library_layout list" sheetId="10" r:id="rId10"/>
+    <sheet name="library_final_yield_unit list" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -37,11 +38,37 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Version of the schema to use when validating this metadata.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Free-text description of this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>HuBMAP Display ID of the donor of the assayed tissue.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="D1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -54,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -106,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -119,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="J1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="K1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -145,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="L1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -158,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -171,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -184,7 +211,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -197,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -210,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="Q1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -223,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="R1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -236,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0">
+    <comment ref="S1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -249,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0">
+    <comment ref="T1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -262,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0">
+    <comment ref="U1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -275,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0">
+    <comment ref="V1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -288,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0">
+    <comment ref="W1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -301,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0">
+    <comment ref="X1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -314,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="W1" authorId="0">
+    <comment ref="Y1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -327,7 +354,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0">
+    <comment ref="Z1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -340,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Y1" authorId="0">
+    <comment ref="AA1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -353,7 +380,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0">
+    <comment ref="AB1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -366,7 +393,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AA1" authorId="0">
+    <comment ref="AC1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +406,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB1" authorId="0">
+    <comment ref="AD1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -392,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC1" authorId="0">
+    <comment ref="AE1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -405,7 +432,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD1" authorId="0">
+    <comment ref="AF1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -418,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE1" authorId="0">
+    <comment ref="AG1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -431,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AF1" authorId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -444,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AG1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -457,7 +484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -470,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -483,7 +510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -496,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +536,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -522,7 +549,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -535,7 +562,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -548,7 +575,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
+    <comment ref="AQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -561,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0">
+    <comment ref="AR1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -574,7 +601,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0">
+    <comment ref="AS1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -592,7 +619,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="66">
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
   <si>
     <t>donor_id</t>
   </si>
@@ -1129,7 +1165,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:AS1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1138,114 +1174,114 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="U1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="AE1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AK1" s="1" t="s">
         <v>56</v>
@@ -1254,85 +1290,94 @@
         <v>57</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="19">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="I2:I1048576">
+  <dataValidations count="20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+      <formula1>'version list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-seq2 / scATACseq / sciATACseq / snATACseq." sqref="J2:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-seq2 / scATACseq / sciATACseq / snATACseq." sqref="L2:L1048576">
       <formula1>'assay_type list'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DNA." sqref="K2:K1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DNA." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="N2:N1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="O2:O1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="Q2:Q1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: whole cell / nucleus / cell-cell multimer / spatially encoded cell barcoding." sqref="R2:R1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: whole cell / nucleus / cell-cell multimer / spatially encoded cell barcoding." sqref="T2:T1048576">
       <formula1>'sc_isolation_entity list'!$A$1:$A$4</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: none / FACS." sqref="T2:T1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: none / FACS." sqref="V2:V1048576">
       <formula1>'sc_isolation_enrichment list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="V2:V1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="X2:X1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="W2:W1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="Y2:Y1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-Seq2-AC / scATACseq / bulkATACseq / snATACseq / sciATACseq." sqref="X2:X1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-Seq2-AC / scATACseq / bulkATACseq / snATACseq / sciATACseq." sqref="Z2:Z1048576">
       <formula1>'transposition_method list'!$A$1:$A$5</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 10X snATAC / In-house / Nextera." sqref="Y2:Y1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 10X snATAC / In-house / Nextera." sqref="AA2:AA1048576">
       <formula1>'transposition_...se_source list'!$A$1:$A$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: single-end / paired-end." sqref="AB2:AB1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: single-end / paired-end." sqref="AD2:AD1048576">
       <formula1>'library_layout list'!$A$1:$A$2</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AG2:AG1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AI2:AI1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AH2:AH1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AJ2:AJ1048576">
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
-      <formula1>-1e+307</formula1>
-      <formula2>1e+307</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AJ2:AJ1048576">
-      <formula1>'library_final_yield_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AK2:AK1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AN2:AN1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AL2:AL1048576">
+      <formula1>'library_final_yield_unit list'!$A$1:$A$1</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AM2:AM1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AO2:AO1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AP2:AP1048576">
+      <formula1>-1e+307</formula1>
+      <formula2>1e+307</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AQ2:AQ1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -1343,6 +1388,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1352,7 +1420,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1370,7 +1438,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1379,6 +1447,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -1388,22 +1474,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1411,7 +1497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1421,7 +1507,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1429,7 +1515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
@@ -1439,22 +1525,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1462,7 +1548,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -1472,12 +1558,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1485,7 +1571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
@@ -1495,27 +1581,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1523,7 +1609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A3"/>
   <sheetViews>
@@ -1533,40 +1619,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mccalluc/factor out fields (#718)
* warn if includes are misused

* replace phix

* sequencing_read_format

* sequencing_reagent_kit

* changelog
</commit_message>
<xml_diff>
--- a/docs/scatacseq/scatacseq-metadata.xlsx
+++ b/docs/scatacseq/scatacseq-metadata.xlsx
@@ -558,7 +558,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Number of sequencing cycles in Read1, i7 index, i5 index, and Read2.</t>
+          <t>Slash-delimited list of the number of sequencing cycles for, for example, Read1, i7 index, i5 index, and Read2.</t>
         </r>
       </text>
     </comment>
@@ -584,7 +584,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Percent PhiX loaded to the run.</t>
+          <t>Percent PhiX loaded to the run</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
fix yaml and regen
</commit_message>
<xml_diff>
--- a/docs/scatacseq/scatacseq-metadata.xlsx
+++ b/docs/scatacseq/scatacseq-metadata.xlsx
@@ -441,7 +441,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Which read file contains the cell barcode.</t>
+          <t>Which read file contains the cell barcode. This field is not required for barcoding by single-cell combinatorial indexing.</t>
         </r>
       </text>
     </comment>
@@ -454,7 +454,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Positions in the read at which the cell barcodes start. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences (the offsets). First barcode at position 0, then 38, then 76. (Does not apply to SNARE-seq and BulkATAC.)</t>
+          <t>Positions in the read at which the cell barcodes start. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences (the offsets). First barcode at position 0, then 38, then 76. (Does not apply to sciATACseq, SNARE-seq and BulkATAC.)</t>
         </r>
       </text>
     </comment>
@@ -467,7 +467,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Length of the cell barcode in base pairs. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences, the offsets. (Does not apply to SNARE-seq and BulkATAC.)</t>
+          <t>Length of the cell barcode in base pairs. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences, the offsets. (Does not apply to sciATACseq, SNARE-seq and BulkATAC.)</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
cell_barcode fields are not required for sciATACseq (#876)
* cell_barcode fields are not required for sciATACseq 

cell_barcode fields are not required for sciATACseq or SNAREseq either (as was already noted in parentheses)
Added required: FALSE for cell_barcode read, index & size

* Update src/ingest_validation_tools/table-schemas/assays/scatacseq-v1.yaml

Co-authored-by: Chuck McCallum <mccalluc@users.noreply.github.com>

* required under constraints

Co-authored-by: chris briggs <cebriggs7135@gmail.com>

* fix yaml and regen

* changelog

* Rerun CI... network problem?

Co-authored-by: Chuck McCallum <mccalluc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/scatacseq/scatacseq-metadata.xlsx
+++ b/docs/scatacseq/scatacseq-metadata.xlsx
@@ -441,7 +441,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Which read file contains the cell barcode.</t>
+          <t>Which read file contains the cell barcode. This field is not required for barcoding by single-cell combinatorial indexing.</t>
         </r>
       </text>
     </comment>
@@ -454,7 +454,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Positions in the read at which the cell barcodes start. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences (the offsets). First barcode at position 0, then 38, then 76. (Does not apply to SNARE-seq and BulkATAC.)</t>
+          <t>Positions in the read at which the cell barcodes start. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences (the offsets). First barcode at position 0, then 38, then 76. (Does not apply to sciATACseq, SNARE-seq and BulkATAC.)</t>
         </r>
       </text>
     </comment>
@@ -467,7 +467,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Length of the cell barcode in base pairs. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences, the offsets. (Does not apply to SNARE-seq and BulkATAC.)</t>
+          <t>Length of the cell barcode in base pairs. Cell barcodes are, for example, 3 x 8 bp sequences that are spaced by constant sequences, the offsets. (Does not apply to sciATACseq, SNARE-seq and BulkATAC.)</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
Clear scATACseq out of the table schemas
</commit_message>
<xml_diff>
--- a/docs/scatacseq/scatacseq-metadata.xlsx
+++ b/docs/scatacseq/scatacseq-metadata.xlsx
@@ -619,7 +619,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>version</t>
   </si>
@@ -664,9 +664,6 @@
   </si>
   <si>
     <t>SNARE-seq2</t>
-  </si>
-  <si>
-    <t>scATACseq</t>
   </si>
   <si>
     <t>sciATACseq</t>
@@ -1215,103 +1212,103 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="AE1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="AM1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1322,8 +1319,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-seq2 / scATACseq / sciATACseq / snATACseq." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-seq2 / sciATACseq / snATACseq." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DNA." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1348,8 +1345,8 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-Seq2-AC / scATACseq / bulkATACseq / snATACseq / sciATACseq." sqref="Z2:Z1048576">
-      <formula1>'transposition_method list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-Seq2-AC / bulkATACseq / snATACseq / sciATACseq." sqref="Z2:Z1048576">
+      <formula1>'transposition_method list'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 10X snATAC / In-house / Nextera / 10X multiome." sqref="AA2:AA1048576">
       <formula1>'transposition_...se_source list'!$A$1:$A$4</formula1>
@@ -1400,12 +1397,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1423,7 +1420,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1469,7 +1466,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1488,11 +1485,6 @@
     <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1502,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1528,22 +1520,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1561,12 +1553,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1568,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1584,27 +1576,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1622,22 +1609,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove snRNA and scATACseq; add Multiplex Ion Beam Imaging (#1040)
* Remove snRNA and scATACseq; add Multiplex Ion Beam Imaging

* Update CHANGELOG

* Clear scATACseq out of the table schemas
</commit_message>
<xml_diff>
--- a/docs/scatacseq/scatacseq-metadata.xlsx
+++ b/docs/scatacseq/scatacseq-metadata.xlsx
@@ -619,7 +619,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>version</t>
   </si>
@@ -664,9 +664,6 @@
   </si>
   <si>
     <t>SNARE-seq2</t>
-  </si>
-  <si>
-    <t>scATACseq</t>
   </si>
   <si>
     <t>sciATACseq</t>
@@ -1215,103 +1212,103 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="U1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="W1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="AE1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AL1" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="AM1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AN1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1322,8 +1319,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-seq2 / scATACseq / sciATACseq / snATACseq." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$4</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-seq2 / sciATACseq / snATACseq." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$3</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: DNA." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1348,8 +1345,8 @@
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-Seq2-AC / scATACseq / bulkATACseq / snATACseq / sciATACseq." sqref="Z2:Z1048576">
-      <formula1>'transposition_method list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: SNARE-Seq2-AC / bulkATACseq / snATACseq / sciATACseq." sqref="Z2:Z1048576">
+      <formula1>'transposition_method list'!$A$1:$A$4</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 10X snATAC / In-house / Nextera / 10X multiome." sqref="AA2:AA1048576">
       <formula1>'transposition_...se_source list'!$A$1:$A$4</formula1>
@@ -1400,12 +1397,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1423,7 +1420,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1469,7 +1466,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1488,11 +1485,6 @@
     <row r="3" spans="1:1">
       <c r="A3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1510,7 +1502,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1528,22 +1520,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1561,12 +1553,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1576,7 +1568,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1584,27 +1576,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1622,22 +1609,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>